<commit_message>
Ajustes na leitura do caracter &
</commit_message>
<xml_diff>
--- a/test/resources/planilhaSimples.xlsx
+++ b/test/resources/planilhaSimples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">(abcdef</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">@Teste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Teste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;Outro &amp;Teste</t>
   </si>
   <si>
     <t xml:space="preserve">“A</t>
@@ -139,8 +145,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,63 +171,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>